<commit_message>
add annotations to category and detail layout templates
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy.fitzgerald/Repos/Content-First-Prototyping/_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="15760" windowHeight="16100" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -250,7 +255,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -440,7 +445,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -449,7 +454,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="6" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -786,7 +791,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -800,14 +805,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="2" max="2" width="30.1640625" customWidth="1"/>
     <col min="3" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
@@ -821,7 +826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
@@ -835,7 +840,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -844,7 +849,7 @@
       </c>
       <c r="C3" s="17"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -853,20 +858,15 @@
       </c>
       <c r="C4" s="17"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C5" s="17"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" s="17"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -878,14 +878,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.1640625" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -896,7 +896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>52</v>
       </c>
@@ -907,7 +907,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>58</v>
       </c>
@@ -915,7 +915,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -926,11 +926,6 @@
   </sheetData>
   <autoFilter ref="A1:C1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -938,12 +933,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="21"/>
     <col min="2" max="2" width="56" style="21" customWidth="1"/>
@@ -965,7 +960,7 @@
     <col min="18" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="19" customFormat="1">
+    <row r="1" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>17</v>
       </c>
@@ -985,7 +980,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="45">
+    <row r="2" spans="1:21" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -1003,7 +998,7 @@
       <c r="K2" s="20"/>
       <c r="M2" s="22"/>
     </row>
-    <row r="3" spans="1:21" ht="45">
+    <row r="3" spans="1:21" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>19</v>
       </c>
@@ -1020,7 +1015,7 @@
       <c r="I3" s="22"/>
       <c r="M3" s="22"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
@@ -1036,7 +1031,7 @@
       </c>
       <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="1:21" ht="60">
+    <row r="5" spans="1:21" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>21</v>
       </c>
@@ -1057,7 +1052,7 @@
       <c r="Q5" s="25"/>
       <c r="U5" s="22"/>
     </row>
-    <row r="6" spans="1:21" ht="45">
+    <row r="6" spans="1:21" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>22</v>
       </c>
@@ -1076,7 +1071,7 @@
       <c r="M6" s="22"/>
       <c r="Q6" s="22"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B7" s="20"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -1086,7 +1081,7 @@
       <c r="M7" s="22"/>
       <c r="Q7" s="22"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B8" s="20"/>
       <c r="D8" s="23"/>
       <c r="E8" s="20"/>
@@ -1094,26 +1089,26 @@
       <c r="M8" s="22"/>
       <c r="Q8" s="22"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="I9" s="22"/>
       <c r="M9" s="22"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B10" s="20"/>
       <c r="E10" s="23"/>
       <c r="I10" s="22"/>
       <c r="M10" s="22"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B11" s="20"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B12" s="27"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
@@ -1121,7 +1116,7 @@
       <c r="M12" s="22"/>
       <c r="Q12" s="22"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B13" s="27"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
@@ -1132,7 +1127,7 @@
       <c r="N13" s="26"/>
       <c r="Q13" s="22"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -1143,7 +1138,7 @@
       <c r="N14" s="26"/>
       <c r="Q14" s="22"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B15" s="20"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
@@ -1152,7 +1147,7 @@
       <c r="J15" s="26"/>
       <c r="M15" s="22"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B16" s="20"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
@@ -1161,7 +1156,7 @@
       <c r="M16" s="22"/>
       <c r="Q16" s="22"/>
     </row>
-    <row r="17" spans="2:21">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B17" s="20"/>
       <c r="D17" s="26"/>
       <c r="I17" s="22"/>
@@ -1172,7 +1167,7 @@
       <c r="Q17" s="25"/>
       <c r="U17" s="22"/>
     </row>
-    <row r="18" spans="2:21" s="20" customFormat="1">
+    <row r="18" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="23"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
@@ -1183,18 +1178,13 @@
       <c r="L18" s="21"/>
       <c r="M18" s="22"/>
     </row>
-    <row r="19" spans="2:21">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B19" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:F6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1202,11 +1192,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="4" customWidth="1"/>
@@ -1229,7 +1219,7 @@
     <col min="20" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1249,7 +1239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1270,7 +1260,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="90">
+    <row r="3" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1291,7 +1281,7 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="65">
+    <row r="4" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1312,95 +1302,90 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="C6" s="4"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1">
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="2:2" s="6" customFormat="1">
+    <row r="17" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="2:2" s="6" customFormat="1">
+    <row r="18" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="2:2" s="6" customFormat="1">
+    <row r="19" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="2:2" s="6" customFormat="1">
+    <row r="20" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="2:2" s="6" customFormat="1">
+    <row r="21" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="2:2" s="6" customFormat="1">
+    <row r="22" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="2:2" s="6" customFormat="1">
+    <row r="23" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="2:2" s="6" customFormat="1">
+    <row r="24" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1412,7 +1397,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="7" customWidth="1"/>
@@ -1421,7 +1406,7 @@
     <col min="5" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1">
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -1435,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>45</v>
       </c>
@@ -1449,7 +1434,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="26">
+    <row r="3" spans="1:4" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>46</v>
       </c>
@@ -1463,7 +1448,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>47</v>
       </c>
@@ -1477,56 +1462,51 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="12"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C14" s="12"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C15" s="12"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C16" s="12"/>
     </row>
-    <row r="17" spans="3:3" s="9" customFormat="1">
+    <row r="17" spans="3:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C17" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
format top nav to pull programmatically from navigation.json
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy.fitzgerald/Repos/Content-First-Prototyping/_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="460" windowWidth="15760" windowHeight="16100" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="860" yWindow="0" windowWidth="22320" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="navigation" sheetId="4" r:id="rId1"/>
@@ -23,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">categories!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">directory!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">feed!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">navigation!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">navigation!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
   <si>
     <t>description</t>
   </si>
@@ -226,9 +221,6 @@
     <t>sub-nav</t>
   </si>
   <si>
-    <t>categories</t>
-  </si>
-  <si>
     <t>specialties</t>
   </si>
   <si>
@@ -248,6 +240,24 @@
   </si>
   <si>
     <t>/tearsheet.html</t>
+  </si>
+  <si>
+    <t>sub-nav-path</t>
+  </si>
+  <si>
+    <t>/catalogue.html</t>
+  </si>
+  <si>
+    <t>/directory.html</t>
+  </si>
+  <si>
+    <t>/feed.html</t>
+  </si>
+  <si>
+    <t>sub-nav-label</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -255,14 +265,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -308,6 +319,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -332,7 +349,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -383,8 +400,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -445,7 +465,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -454,7 +474,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -473,8 +493,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -502,6 +525,9 @@
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -791,7 +817,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -799,34 +825,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="2" max="2" width="30.1640625" customWidth="1"/>
-    <col min="3" max="4" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>62</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
@@ -834,39 +867,99 @@
         <v>13</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>57</v>
       </c>
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="17"/>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:F1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -875,17 +968,17 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="38.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.1640625" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -896,7 +989,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
         <v>52</v>
       </c>
@@ -907,7 +1000,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="16" t="s">
         <v>58</v>
       </c>
@@ -915,7 +1008,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -926,6 +1019,12 @@
   </sheetData>
   <autoFilter ref="A1:C1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -938,7 +1037,7 @@
       <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="21"/>
     <col min="2" max="2" width="56" style="21" customWidth="1"/>
@@ -960,7 +1059,7 @@
     <col min="18" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="19" customFormat="1">
       <c r="A1" s="18" t="s">
         <v>17</v>
       </c>
@@ -977,10 +1076,10 @@
         <v>11</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="48" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="48">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -998,7 +1097,7 @@
       <c r="K2" s="20"/>
       <c r="M2" s="22"/>
     </row>
-    <row r="3" spans="1:21" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="48">
       <c r="A3" s="20" t="s">
         <v>19</v>
       </c>
@@ -1015,7 +1114,7 @@
       <c r="I3" s="22"/>
       <c r="M3" s="22"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
@@ -1031,7 +1130,7 @@
       </c>
       <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="1:21" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="64">
       <c r="A5" s="20" t="s">
         <v>21</v>
       </c>
@@ -1052,7 +1151,7 @@
       <c r="Q5" s="25"/>
       <c r="U5" s="22"/>
     </row>
-    <row r="6" spans="1:21" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="48">
       <c r="A6" s="20" t="s">
         <v>22</v>
       </c>
@@ -1071,7 +1170,7 @@
       <c r="M6" s="22"/>
       <c r="Q6" s="22"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21">
       <c r="B7" s="20"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -1081,7 +1180,7 @@
       <c r="M7" s="22"/>
       <c r="Q7" s="22"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21">
       <c r="B8" s="20"/>
       <c r="D8" s="23"/>
       <c r="E8" s="20"/>
@@ -1089,26 +1188,26 @@
       <c r="M8" s="22"/>
       <c r="Q8" s="22"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21">
       <c r="B9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="I9" s="22"/>
       <c r="M9" s="22"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21">
       <c r="B10" s="20"/>
       <c r="E10" s="23"/>
       <c r="I10" s="22"/>
       <c r="M10" s="22"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21">
       <c r="B11" s="20"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21">
       <c r="B12" s="27"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
@@ -1116,7 +1215,7 @@
       <c r="M12" s="22"/>
       <c r="Q12" s="22"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21">
       <c r="B13" s="27"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
@@ -1127,7 +1226,7 @@
       <c r="N13" s="26"/>
       <c r="Q13" s="22"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21">
       <c r="B14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -1138,7 +1237,7 @@
       <c r="N14" s="26"/>
       <c r="Q14" s="22"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21">
       <c r="B15" s="20"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
@@ -1147,7 +1246,7 @@
       <c r="J15" s="26"/>
       <c r="M15" s="22"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21">
       <c r="B16" s="20"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
@@ -1156,7 +1255,7 @@
       <c r="M16" s="22"/>
       <c r="Q16" s="22"/>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:21">
       <c r="B17" s="20"/>
       <c r="D17" s="26"/>
       <c r="I17" s="22"/>
@@ -1167,7 +1266,7 @@
       <c r="Q17" s="25"/>
       <c r="U17" s="22"/>
     </row>
-    <row r="18" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:21" s="20" customFormat="1">
       <c r="B18" s="23"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
@@ -1178,13 +1277,18 @@
       <c r="L18" s="21"/>
       <c r="M18" s="22"/>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:21">
       <c r="B19" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:F6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1192,11 +1296,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="4" customWidth="1"/>
@@ -1219,7 +1323,7 @@
     <col min="20" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1233,13 +1337,13 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="48">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1253,14 +1357,14 @@
         <v>37</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="96">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1274,14 +1378,14 @@
         <v>38</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>54</v>
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="56">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1295,97 +1399,102 @@
         <v>39</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>54</v>
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="B6" s="5"/>
       <c r="C6" s="4"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="B9" s="5"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="B10" s="5"/>
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" s="6" customFormat="1">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" s="6" customFormat="1">
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" s="6" customFormat="1">
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" s="6" customFormat="1">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" s="6" customFormat="1">
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" s="6" customFormat="1">
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" s="6" customFormat="1">
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" s="6" customFormat="1">
       <c r="B24" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1397,7 +1506,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="7" customWidth="1"/>
@@ -1406,7 +1515,7 @@
     <col min="5" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="11" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -1420,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>45</v>
       </c>
@@ -1434,7 +1543,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="28">
       <c r="A3" s="7" t="s">
         <v>46</v>
       </c>
@@ -1448,7 +1557,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="32">
       <c r="A4" s="7" t="s">
         <v>47</v>
       </c>
@@ -1462,51 +1571,56 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="B5" s="5"/>
       <c r="C5" s="12"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="B6" s="5"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="C14" s="12"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="C15" s="12"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="C16" s="12"/>
     </row>
-    <row r="17" spans="3:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" s="9" customFormat="1">
       <c r="C17" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add "instructions" tab to _data.xlsx
</commit_message>
<xml_diff>
--- a/_data/_data.xlsx
+++ b/_data/_data.xlsx
@@ -7,18 +7,19 @@
     <workbookView xWindow="860" yWindow="0" windowWidth="22320" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="navigation" sheetId="4" r:id="rId1"/>
-    <sheet name="categories" sheetId="5" r:id="rId2"/>
-    <sheet name="catalogue" sheetId="1" r:id="rId3"/>
-    <sheet name="directory" sheetId="3" r:id="rId4"/>
-    <sheet name="feed" sheetId="2" r:id="rId5"/>
+    <sheet name="!_Instructions" sheetId="6" r:id="rId1"/>
+    <sheet name="navigation" sheetId="4" r:id="rId2"/>
+    <sheet name="categories" sheetId="5" r:id="rId3"/>
+    <sheet name="catalogue" sheetId="1" r:id="rId4"/>
+    <sheet name="directory" sheetId="3" r:id="rId5"/>
+    <sheet name="feed" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">catalogue!$B$1:$F$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">categories!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">directory!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">feed!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">navigation!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">catalogue!$B$1:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">categories!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">directory!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">feed!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">navigation!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -825,9 +826,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -963,12 +983,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1028,7 +1048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
@@ -1292,7 +1312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
@@ -1498,7 +1518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>

</xml_diff>